<commit_message>
Performed experiments with all FS methods.
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -351,15 +351,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D12"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B12"/>
+      <selection activeCell="E3" sqref="E3:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -370,114 +370,144 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
+        <v>0.77906976744186052</v>
+      </c>
+      <c r="C3">
+        <v>0.81395348837209303</v>
+      </c>
+      <c r="D3">
+        <v>0.87209302325581395</v>
+      </c>
+      <c r="E3">
+        <v>0.87209302325581395</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.72941176470588232</v>
+      </c>
+      <c r="C4">
+        <v>0.74117647058823533</v>
+      </c>
+      <c r="D4">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="E4">
+        <v>0.81176470588235294</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="C5">
+        <v>0.71764705882352942</v>
+      </c>
+      <c r="D5">
+        <v>0.77647058823529413</v>
+      </c>
+      <c r="E5">
+        <v>0.81176470588235294</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="C6">
+        <v>0.8</v>
+      </c>
+      <c r="D6">
+        <v>0.87058823529411766</v>
+      </c>
+      <c r="E6">
+        <v>0.87058823529411766</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.8</v>
+      </c>
+      <c r="C7">
+        <v>0.77647058823529413</v>
+      </c>
+      <c r="D7">
+        <v>0.87058823529411766</v>
+      </c>
+      <c r="E7">
+        <v>0.88235294117647056</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.86046511627906974</v>
+      </c>
+      <c r="C8">
+        <v>0.86046511627906974</v>
+      </c>
+      <c r="D8">
+        <v>0.89534883720930236</v>
+      </c>
+      <c r="E8">
+        <v>0.89534883720930236</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.77906976744186052</v>
+      </c>
+      <c r="C9">
+        <v>0.83720930232558144</v>
+      </c>
+      <c r="D9">
+        <v>0.87209302325581395</v>
+      </c>
+      <c r="E9">
+        <v>0.88372093023255816</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.79069767441860461</v>
+      </c>
+      <c r="C10">
+        <v>0.80232558139534882</v>
+      </c>
+      <c r="D10">
         <v>0.84883720930232553</v>
       </c>
-      <c r="C3">
-        <v>0.87209302325581395</v>
-      </c>
-      <c r="D3">
-        <v>0.88372093023255816</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>0.82352941176470584</v>
-      </c>
-      <c r="C4">
-        <v>0.89411764705882357</v>
-      </c>
-      <c r="D4">
-        <v>0.89411764705882357</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>0.82352941176470584</v>
-      </c>
-      <c r="C5">
-        <v>0.85882352941176465</v>
-      </c>
-      <c r="D5">
-        <v>0.87058823529411766</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>0.91764705882352937</v>
-      </c>
-      <c r="C6">
-        <v>0.76470588235294112</v>
-      </c>
-      <c r="D6">
-        <v>0.77647058823529413</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>0.85882352941176465</v>
-      </c>
-      <c r="C7">
-        <v>0.85882352941176465</v>
-      </c>
-      <c r="D7">
-        <v>0.82352941176470584</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8">
+      <c r="E10">
+        <v>0.86046511627906974</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.76744186046511631</v>
+      </c>
+      <c r="C11">
+        <v>0.77906976744186052</v>
+      </c>
+      <c r="D11">
         <v>0.82558139534883723</v>
       </c>
-      <c r="C8">
-        <v>0.87209302325581395</v>
-      </c>
-      <c r="D8">
-        <v>0.87209302325581395</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>0.87209302325581395</v>
-      </c>
-      <c r="C9">
+      <c r="E11">
         <v>0.81395348837209303</v>
       </c>
-      <c r="D9">
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0.81395348837209303</v>
+      </c>
+      <c r="C12">
         <v>0.82558139534883723</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>0.83720930232558144</v>
-      </c>
-      <c r="C10">
-        <v>0.82558139534883723</v>
-      </c>
-      <c r="D10">
-        <v>0.82558139534883723</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>0.86046511627906974</v>
-      </c>
-      <c r="C11">
-        <v>0.90697674418604646</v>
-      </c>
-      <c r="D11">
-        <v>0.88372093023255816</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>0.86046511627906974</v>
-      </c>
-      <c r="C12">
-        <v>0.84883720930232553</v>
       </c>
       <c r="D12">
         <v>0.86046511627906974</v>
+      </c>
+      <c r="E12">
+        <v>0.83720930232558144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extended experiments with SVM. Added NN comparsion. Updated calculations file (.xlsx).
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -21,20 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>6 features</t>
-  </si>
-  <si>
-    <t>12 features</t>
-  </si>
-  <si>
-    <t>20 features</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -351,163 +337,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>0.77906976744186052</v>
-      </c>
-      <c r="C3">
-        <v>0.81395348837209303</v>
-      </c>
-      <c r="D3">
-        <v>0.87209302325581395</v>
-      </c>
-      <c r="E3">
-        <v>0.87209302325581395</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.72789329685362536</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>0.72941176470588232</v>
-      </c>
-      <c r="C4">
-        <v>0.74117647058823533</v>
-      </c>
-      <c r="D4">
-        <v>0.82352941176470584</v>
-      </c>
-      <c r="E4">
-        <v>0.81176470588235294</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.78281805745554023</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>0.70588235294117652</v>
-      </c>
-      <c r="C5">
-        <v>0.71764705882352942</v>
-      </c>
-      <c r="D5">
-        <v>0.77647058823529413</v>
-      </c>
-      <c r="E5">
-        <v>0.81176470588235294</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.78050615595075234</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>0.76470588235294112</v>
-      </c>
-      <c r="C6">
-        <v>0.8</v>
-      </c>
-      <c r="D6">
-        <v>0.87058823529411766</v>
-      </c>
-      <c r="E6">
-        <v>0.87058823529411766</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.78748290013679889</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>0.8</v>
-      </c>
-      <c r="C7">
-        <v>0.77647058823529413</v>
-      </c>
-      <c r="D7">
-        <v>0.87058823529411766</v>
-      </c>
-      <c r="E7">
-        <v>0.88235294117647056</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.79098495212038311</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>0.86046511627906974</v>
-      </c>
-      <c r="C8">
-        <v>0.86046511627906974</v>
-      </c>
-      <c r="D8">
-        <v>0.89534883720930236</v>
-      </c>
-      <c r="E8">
-        <v>0.89534883720930236</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.79564979480164166</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>0.77906976744186052</v>
-      </c>
-      <c r="C9">
-        <v>0.83720930232558144</v>
-      </c>
-      <c r="D9">
-        <v>0.87209302325581395</v>
-      </c>
-      <c r="E9">
-        <v>0.88372093023255816</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.79564979480164166</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>0.79069767441860461</v>
-      </c>
-      <c r="C10">
-        <v>0.80232558139534882</v>
-      </c>
-      <c r="D10">
-        <v>0.84883720930232553</v>
-      </c>
-      <c r="E10">
-        <v>0.86046511627906974</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.79564979480164166</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>0.76744186046511631</v>
-      </c>
-      <c r="C11">
-        <v>0.77906976744186052</v>
-      </c>
-      <c r="D11">
-        <v>0.82558139534883723</v>
-      </c>
-      <c r="E11">
-        <v>0.81395348837209303</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+        <v>0.8459097127222982</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>0.81395348837209303</v>
-      </c>
-      <c r="C12">
-        <v>0.82558139534883723</v>
-      </c>
-      <c r="D12">
-        <v>0.86046511627906974</v>
-      </c>
-      <c r="E12">
-        <v>0.83720930232558144</v>
+        <v>0.84824897400820787</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0.85058823529411764</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0.84826265389876865</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0.84826265389876865</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0.84945280437756487</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0.85644322845417231</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0.86231190150478787</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.86231190150478787</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0.85294117647058809</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.85177838577291376</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>3.8120610483515317E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>4.0899756429051339E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>4.5192447831820665E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>4.8691155096905525E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>5.1569798576955782E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>5.2718889773369672E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>5.2718889773369672E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>5.2718889773369672E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>4.8029479058413975E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>4.3196746468155342E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>4.6149435157906843E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>4.6475930258191342E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>4.6475930258191342E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>4.9145671896234797E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>4.4531269255142752E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>4.2692133359570353E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>4.2692133359570353E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>3.2436440789482546E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>4.0979347162469794E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>0.21481203579188118</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>0.20945374962015989</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>0.17524799366348637</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>0.19097187608880026</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>0.27589316502865024</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>0.25646672805548237</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>0.26655103143706405</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>0.25534762376899167</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>0.25002970880760544</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>0.21667848106969112</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>0.30262446147186212</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>0.24315265104707867</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>0.28635360930652393</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>0.28741547197836081</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>0.28960294133835296</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>0.29557877646816677</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>0.29121484575100048</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>0.30813276368198755</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>0.3332250709056182</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>0.33486244732478648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>